<commit_message>
added year and section
</commit_message>
<xml_diff>
--- a/CAI/bin/Debug/templates/TestTemplate.xlsx
+++ b/CAI/bin/Debug/templates/TestTemplate.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">SAINT JEAN BAPTISTE ACADEMY
 BALIUAG, BULACAN
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Year &amp; Section</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -396,6 +399,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -423,11 +461,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -452,9 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -485,6 +517,18 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Currency 2" xfId="10"/>
@@ -914,122 +958,123 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="2"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>